<commit_message>
Simulator loopback functional test
</commit_message>
<xml_diff>
--- a/examples/AN00162_i2s_loopback_demo/backpressure tolerance i2s.xlsx
+++ b/examples/AN00162_i2s_loopback_demo/backpressure tolerance i2s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1360" yWindow="80" windowWidth="31040" windowHeight="18620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nice graph" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="12">
   <si>
     <t>Backpressure_test_results.txt</t>
   </si>
@@ -56,15 +56,34 @@
   <si>
     <t>ADDITIONAL_SERVER_CASE 1</t>
   </si>
+  <si>
+    <t>Adjusted for channel count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,13 +106,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -793,6 +820,184 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Block transfer</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Two halves'!$I$2:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>254.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>123.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>61.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28.75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Block transfer + SERVER</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Two halves'!$I$28:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.16666666666667</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.875</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -871,8 +1076,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -1222,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -3935,20 +4140,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3973,8 +4184,12 @@
       <c r="H2">
         <v>509</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f>H2/(2*D2)</f>
+        <v>254.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3999,8 +4214,12 @@
       <c r="H3">
         <v>506</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="0">H3/(2*D3)</f>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4025,8 +4244,12 @@
       <c r="H4">
         <v>501</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>250.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4051,8 +4274,12 @@
       <c r="H5">
         <v>504</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4077,8 +4304,12 @@
       <c r="H6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4103,8 +4334,12 @@
       <c r="H7">
         <v>493</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4129,8 +4364,12 @@
       <c r="H8">
         <v>489</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4155,8 +4394,12 @@
       <c r="H9">
         <v>484</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>80.666666666666671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4181,8 +4424,12 @@
       <c r="H10">
         <v>474</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4207,8 +4454,12 @@
       <c r="H11">
         <v>485</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>60.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -4233,8 +4484,12 @@
       <c r="H12">
         <v>479</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>59.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -4259,8 +4514,12 @@
       <c r="H13">
         <v>465</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>58.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -4285,8 +4544,12 @@
       <c r="H14">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -4311,8 +4574,12 @@
       <c r="H15">
         <v>247</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -4337,8 +4604,12 @@
       <c r="H16">
         <v>242</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4363,8 +4634,12 @@
       <c r="H17">
         <v>245</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -4389,8 +4664,12 @@
       <c r="H18">
         <v>240</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4415,8 +4694,12 @@
       <c r="H19">
         <v>233</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>58.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4441,8 +4724,12 @@
       <c r="H20">
         <v>231</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4467,8 +4754,12 @@
       <c r="H21">
         <v>228</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4493,8 +4784,12 @@
       <c r="H22">
         <v>218</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>36.333333333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4519,8 +4814,12 @@
       <c r="H23">
         <v>230</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>28.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -4545,8 +4844,12 @@
       <c r="H24">
         <v>224</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -4571,13 +4874,17 @@
       <c r="H25">
         <v>210</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -4602,8 +4909,12 @@
       <c r="H28">
         <v>466</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <f>H28/(2*D28)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4628,8 +4939,12 @@
       <c r="H29">
         <v>454</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <f t="shared" ref="I29:I51" si="1">H29/(2*D29)</f>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -4654,8 +4969,12 @@
       <c r="H30">
         <v>432</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4680,8 +4999,12 @@
       <c r="H31">
         <v>461</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>115.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -4706,8 +5029,12 @@
       <c r="H32">
         <v>448</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -4732,8 +5059,12 @@
       <c r="H33">
         <v>423</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>105.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -4758,8 +5089,12 @@
       <c r="H34">
         <v>446</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>74.333333333333329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -4784,8 +5119,12 @@
       <c r="H35">
         <v>432</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -4810,8 +5149,12 @@
       <c r="H36">
         <v>405</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -4836,8 +5179,12 @@
       <c r="H37">
         <v>438</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>54.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -4862,8 +5209,12 @@
       <c r="H38">
         <v>422</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>52.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -4888,8 +5239,12 @@
       <c r="H39">
         <v>393</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>49.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -4914,8 +5269,12 @@
       <c r="H40">
         <v>207</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -4940,8 +5299,12 @@
       <c r="H41">
         <v>195</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -4966,8 +5329,12 @@
       <c r="H42">
         <v>172</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -4992,8 +5359,12 @@
       <c r="H43">
         <v>202</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -5018,8 +5389,12 @@
       <c r="H44">
         <v>189</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>47.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -5044,8 +5419,12 @@
       <c r="H45">
         <v>165</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -5070,8 +5449,12 @@
       <c r="H46">
         <v>189</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -5096,8 +5479,12 @@
       <c r="H47">
         <v>175</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>29.166666666666668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -5122,8 +5509,12 @@
       <c r="H48">
         <v>148</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>24.666666666666668</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -5148,8 +5539,12 @@
       <c r="H49">
         <v>182</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -5174,8 +5569,12 @@
       <c r="H50">
         <v>167</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>20.875</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -5200,9 +5599,14 @@
       <c r="H51">
         <v>68</v>
       </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5213,12 +5617,642 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>96000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>96000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>96000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>96000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>96000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>96000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>96000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>96000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>96000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>96000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>96000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>96000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>192000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>192000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>192000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>192000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>192000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>192000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>192000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>192000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>192000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>192000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>192000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>192000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>